<commit_message>
dilution term added. We approach closer
</commit_message>
<xml_diff>
--- a/input/calorimetry/test_5.xlsx
+++ b/input/calorimetry/test_5.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>lg_k</t>
   </si>
@@ -1082,10 +1082,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,6 +1098,14 @@
         <v>10</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
writing to file fixed
</commit_message>
<xml_diff>
--- a/input/calorimetry/test_5.xlsx
+++ b/input/calorimetry/test_5.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="input_k_constants_log10" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="enthalpies" sheetId="7" r:id="rId7"/>
     <sheet name="setup" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -417,7 +417,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,7 +681,7 @@
   <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,64 +821,64 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>2.239E-2</v>
+        <v>2.2414656273280341E-2</v>
       </c>
       <c r="C3">
-        <v>2.1590000000000002E-2</v>
+        <v>2.1607921114904838E-2</v>
       </c>
       <c r="D3">
-        <v>2.0420000000000001E-2</v>
+        <v>2.043886294103122E-2</v>
       </c>
       <c r="E3">
-        <v>1.8780000000000002E-2</v>
+        <v>1.878770260144811E-2</v>
       </c>
       <c r="F3">
-        <v>1.661E-2</v>
+        <v>1.6619828615365491E-2</v>
       </c>
       <c r="G3">
-        <v>1.4120000000000001E-2</v>
+        <v>1.4117609576194113E-2</v>
       </c>
       <c r="H3">
-        <v>1.167E-2</v>
+        <v>1.1667268720085147E-2</v>
       </c>
       <c r="I3">
-        <v>9.6100000000000005E-3</v>
+        <v>9.6095223315943324E-3</v>
       </c>
       <c r="J3">
-        <v>8.0499999999999999E-3</v>
+        <v>8.0515033120730772E-3</v>
       </c>
       <c r="K3">
-        <v>6.9300000000000004E-3</v>
+        <v>6.9244672048729815E-3</v>
       </c>
       <c r="L3">
-        <v>6.11E-3</v>
+        <v>6.1116789976356639E-3</v>
       </c>
       <c r="M3">
-        <v>5.5100000000000001E-3</v>
+        <v>5.513444381037679E-3</v>
       </c>
       <c r="N3">
-        <v>5.0600000000000003E-3</v>
+        <v>5.0596010678025157E-3</v>
       </c>
       <c r="O3">
-        <v>4.7000000000000002E-3</v>
+        <v>4.7039372883214917E-3</v>
       </c>
       <c r="P3">
-        <v>4.4200000000000003E-3</v>
+        <v>4.4164727744528945E-3</v>
       </c>
       <c r="Q3">
-        <v>4.1799999999999997E-3</v>
+        <v>4.1775888830205251E-3</v>
       </c>
       <c r="R3">
-        <v>3.9699999999999996E-3</v>
+        <v>3.9742994360578831E-3</v>
       </c>
       <c r="S3">
-        <v>3.8E-3</v>
+        <v>3.7977179283120556E-3</v>
       </c>
       <c r="T3">
-        <v>3.64E-3</v>
+        <v>3.6417052714977274E-3</v>
       </c>
       <c r="U3">
-        <v>3.5000000000000001E-3</v>
+        <v>3.5018980113836343E-3</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -1020,7 +1020,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M27" sqref="M26:M27"/>
     </sheetView>
   </sheetViews>
@@ -1094,7 +1094,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>

</xml_diff>